<commit_message>
Added responsibility for working packages
</commit_message>
<xml_diff>
--- a/Documents/Arbeitsaufteilung.xlsx
+++ b/Documents/Arbeitsaufteilung.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="15510" windowHeight="8805"/>
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$I$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$I$24</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>work package</t>
   </si>
@@ -49,13 +49,67 @@
   </si>
   <si>
     <t>Traxler</t>
+  </si>
+  <si>
+    <t>UML Klassendiagramm</t>
+  </si>
+  <si>
+    <t>UML Aktivitätsdiagramm</t>
+  </si>
+  <si>
+    <t>UML Use-Case</t>
+  </si>
+  <si>
+    <t>UML überprüfen</t>
+  </si>
+  <si>
+    <t>Analytics-Server implementieren</t>
+  </si>
+  <si>
+    <t>Billing-Server implementieren</t>
+  </si>
+  <si>
+    <t>Management-Client impl.</t>
+  </si>
+  <si>
+    <t>Testing Component impl.</t>
+  </si>
+  <si>
+    <t>Model-Klassen (Events, Bill, Steps)</t>
+  </si>
+  <si>
+    <t>Refactoring old Source</t>
+  </si>
+  <si>
+    <t>Analytics Unit testen</t>
+  </si>
+  <si>
+    <t>Billing Unit testen</t>
+  </si>
+  <si>
+    <t>Management-Client Unit testen</t>
+  </si>
+  <si>
+    <t>Testing Component Unit testen</t>
+  </si>
+  <si>
+    <t>Protokoll</t>
+  </si>
+  <si>
+    <t>File-Persistence</t>
+  </si>
+  <si>
+    <t>RMI-Verbindungen testen</t>
+  </si>
+  <si>
+    <t>RMI-Verbindungen implementieren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +138,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -234,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -251,27 +311,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -287,7 +350,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -361,6 +424,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -395,6 +459,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -570,48 +635,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <pane xSplit="3855" topLeftCell="D1" activePane="topRight"/>
+      <selection activeCell="A15" sqref="A15"/>
+      <selection pane="topRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="9" width="7.140625" customWidth="1"/>
+    <col min="1" max="2" width="33" customWidth="1"/>
+    <col min="3" max="9" width="7.140625" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" customWidth="1"/>
     <col min="11" max="11" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="7"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -643,35 +710,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="2"/>
       <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="4"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B4" s="4"/>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="2"/>
       <c r="H4" s="4"/>
       <c r="I4" s="2"/>
       <c r="J4" s="4"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="15"/>
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
@@ -682,86 +755,100 @@
       <c r="J5" s="4"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="2"/>
       <c r="J6" s="4"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="4"/>
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="2"/>
       <c r="J7" s="4"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="2"/>
       <c r="H9" s="4"/>
       <c r="I9" s="2"/>
       <c r="J9" s="4"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="2"/>
       <c r="H10" s="4"/>
       <c r="I10" s="2"/>
       <c r="J10" s="4"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A11" s="3"/>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="2"/>
       <c r="J11" s="4"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
@@ -773,9 +860,11 @@
       <c r="J12" s="4"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
       <c r="E13" s="2"/>
@@ -786,9 +875,11 @@
       <c r="J13" s="4"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="2"/>
       <c r="D14" s="4"/>
       <c r="E14" s="2"/>
@@ -796,11 +887,13 @@
       <c r="G14" s="2"/>
       <c r="H14" s="4"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
       <c r="D15" s="4"/>
@@ -809,27 +902,31 @@
       <c r="G15" s="2"/>
       <c r="H15" s="4"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="15"/>
       <c r="C16" s="2"/>
       <c r="D16" s="4"/>
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="15"/>
       <c r="I16" s="2"/>
       <c r="J16" s="4"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="B17" s="4"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="2"/>
       <c r="F17" s="4"/>
       <c r="G17" s="2"/>
@@ -838,46 +935,52 @@
       <c r="J17" s="4"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A18" s="3"/>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" s="4"/>
       <c r="C18" s="2"/>
       <c r="D18" s="4"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="2"/>
       <c r="H18" s="4"/>
       <c r="I18" s="2"/>
       <c r="J18" s="4"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="B19" s="4"/>
       <c r="C19" s="2"/>
       <c r="D19" s="4"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="2"/>
       <c r="H19" s="4"/>
       <c r="I19" s="2"/>
       <c r="J19" s="4"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="15"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="15"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="4"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="2"/>
@@ -890,47 +993,73 @@
       <c r="J21" s="4"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A23" s="11" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="12">
-        <f>SUM(B22,D22,F22,H22,J22)</f>
+      <c r="B25" s="9">
+        <f>SUM(B24,D24,F24,H24,J24)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="12">
-        <f>SUM(C22,E22,G22,I22,K22)</f>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="9">
+        <f>SUM(C24,E24,G24,I24,K24)</f>
         <v>0</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="G25:K25"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -943,24 +1072,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12 new, seperate activity diagrams (see activitydiagramV2.asta)
</commit_message>
<xml_diff>
--- a/Documents/Arbeitsaufteilung.xlsx
+++ b/Documents/Arbeitsaufteilung.xlsx
@@ -15,6 +15,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Tabelle1!$A$1:$I$24</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Tabelle1!$A$1:$I$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Tabelle1!$A$1:$I$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -122,33 +123,33 @@
   </numFmts>
   <fonts count="5">
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -180,29 +181,29 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
       <left/>
-      <right style="medium"/>
+      <right style="thick"/>
       <top/>
-      <bottom style="medium"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
+      <left style="thick"/>
+      <right style="thick"/>
       <top/>
-      <bottom style="medium"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
       <left/>
-      <right style="medium"/>
+      <right style="thick"/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -362,18 +363,18 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" state="split" topLeftCell="B1" xSplit="3717" ySplit="0"/>
-      <selection activeCell="A26" activeCellId="0" pane="topLeft" sqref="A26"/>
-      <selection activeCell="B1" activeCellId="0" pane="topRight" sqref="B1"/>
+      <pane activePane="topRight" topLeftCell="B1" xSplit="3981" ySplit="0"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="G29" activeCellId="0" pane="topRight" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="7.14795918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.56632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.71428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.7295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="7.1497975708502"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.57085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.7246963562753"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="1">
@@ -474,7 +475,9 @@
       <c r="F4" s="5" t="n">
         <v>2.5</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="2"/>
       <c r="J4" s="4"/>
@@ -960,7 +963,7 @@
       </c>
       <c r="G24" s="8" t="n">
         <f aca="false">SUM(G3:G23)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" s="8" t="n">
         <f aca="false">SUM(H3:H23)</f>
@@ -993,7 +996,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="n">
         <f aca="false">SUM(C24,E24,G24,I24,K24)</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
@@ -1064,7 +1067,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7246963562753"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1090,7 +1093,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7246963562753"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Changed USeCase (removed extends)
</commit_message>
<xml_diff>
--- a/Documents/Arbeitsaufteilung.xlsx
+++ b/Documents/Arbeitsaufteilung.xlsx
@@ -221,10 +221,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -249,6 +245,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -621,7 +621,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,664 +634,666 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="1">
         <v>1.5</v>
       </c>
-      <c r="D3" s="6">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="6">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
         <v>4</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="10">
         <v>0.3</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="5">
         <f>L3/2</f>
         <v>0.15</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="6">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="4">
         <v>2.5</v>
       </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="12">
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="10">
         <v>0.25</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="5">
         <f>L4/1</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>0.5</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="12">
+      <c r="D5" s="3"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="10">
         <v>0.2</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="5">
         <f>L5/1</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4">
         <v>0.5</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="12">
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="10">
         <v>0.15</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="5">
         <f>L6/1</f>
         <v>0.15</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="6">
+      <c r="C7" s="1"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="4">
         <v>3</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="12">
+      <c r="I7" s="1"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="10">
         <v>1</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="5">
         <f>L7/2</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="4">
         <v>6</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="6">
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4">
         <v>4</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="12">
+      <c r="K8" s="1"/>
+      <c r="L8" s="10">
         <v>1</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="5">
         <f>L8/2</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="6">
+      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="4">
         <v>3</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="6">
+      <c r="G9" s="1"/>
+      <c r="H9" s="4">
         <v>3</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="12">
+      <c r="I9" s="1"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="10">
         <v>0.65</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="5">
         <f>L9/2</f>
         <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6">
+      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4">
         <v>4</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="12">
+      <c r="G10" s="1"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="10">
         <v>0.5</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="5">
         <f>L10/1</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="6">
+      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="4">
         <v>1.5</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="12">
+      <c r="I11" s="1"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="10">
         <v>0.25</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="5">
         <f>L11/1</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="6">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="12">
+      <c r="B12" s="3"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="10">
         <v>0.25</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="5">
         <f>L12/1</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="6">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="12">
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="4">
+        <v>2</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="10">
         <v>0.4</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="5">
         <f>L13/2</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>1.5</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="6">
+      <c r="C14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="4">
         <v>3</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="12">
+      <c r="K14" s="1"/>
+      <c r="L14" s="10">
         <v>0.8</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="5">
         <f>L14/2</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="6">
+      <c r="B15" s="3"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4">
         <v>1</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="6">
+      <c r="E15" s="1"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="4">
         <v>1</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="12">
+      <c r="K15" s="1"/>
+      <c r="L15" s="10">
         <v>0.5</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="5">
         <f>L15/2</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="6">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="12">
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="4">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="10">
         <v>0.4</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="5">
         <f>L16/2</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="12">
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="10">
         <v>0.4</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="5">
         <f>L17/1</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="6">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="12">
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="4">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="10">
         <v>0.25</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="5">
         <f>L18/1</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="6">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="12">
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="4">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="10">
         <v>0.33</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="5">
         <f>L19/1</f>
         <v>0.33</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="6">
-        <v>2</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="6">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="6">
+      <c r="B20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="6">
+      <c r="G20" s="1"/>
+      <c r="H20" s="4">
         <v>1</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="6">
+      <c r="I20" s="1"/>
+      <c r="J20" s="4">
         <v>1</v>
       </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="12">
+      <c r="K20" s="1"/>
+      <c r="L20" s="10">
         <v>0.4</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="5">
         <f>L20/4</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <f t="shared" ref="B24:K24" si="0">SUM(B3:B23)</f>
         <v>14.5</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D24" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D24" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="7">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="12">
         <f>SUM(B24,D24,F24,H24,J24)</f>
         <v>68</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12">
         <f>SUM(C24,E24,G24,I24,K24)</f>
-        <v>8</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <f>M5+M13+M14+M16+M20+M7</f>
         <v>1.6</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10">
         <f>M3+M8+M17+M20+M15</f>
         <v>1.4000000000000001</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12">
+      <c r="E26" s="10"/>
+      <c r="F26" s="10">
         <f>M4+M9+M10+M18+M19+M20</f>
         <v>1.7550000000000001</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12">
+      <c r="G26" s="10"/>
+      <c r="H26" s="10">
         <f>M6+M7+M11+M16+M20+M9+M12</f>
         <v>1.7750000000000001</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12">
+      <c r="I26" s="10"/>
+      <c r="J26" s="10">
         <f>M3+M8+M14+M15+M20+M13</f>
         <v>1.6</v>
       </c>
-      <c r="K26" s="11"/>
+      <c r="K26" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
time table and protocol (how to save price steps)
</commit_message>
<xml_diff>
--- a/Documents/Arbeitsaufteilung.xlsx
+++ b/Documents/Arbeitsaufteilung.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="113"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$I$24</definedName>
     <definedName name="Print_Area_0" localSheetId="0">Tabelle1!$A$1:$I$24</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -115,8 +115,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -249,6 +249,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -332,7 +335,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -406,7 +409,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -441,7 +443,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -617,14 +618,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33"/>
     <col min="2" max="9" width="7.140625"/>
@@ -633,7 +634,7 @@
     <col min="12" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -658,7 +659,7 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="11"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -694,7 +695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -724,7 +725,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -750,7 +751,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -776,7 +777,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -800,7 +801,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -826,7 +827,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -835,7 +836,9 @@
       <c r="D8" s="4">
         <v>6</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="1"/>
       <c r="H8" s="3"/>
@@ -852,7 +855,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -878,7 +881,7 @@
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -902,7 +905,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -926,7 +929,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -950,7 +953,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -978,7 +981,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="17.25" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1065,7 +1068,9 @@
       <c r="D17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="13">
+        <v>0.5</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="1"/>
       <c r="H17" s="3"/>
@@ -1080,7 +1085,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1104,7 +1109,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1128,7 +1133,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1139,7 +1144,9 @@
       <c r="D20" s="4">
         <v>2</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <v>0.1</v>
+      </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
@@ -1160,7 +1167,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
@@ -1173,7 +1180,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="1"/>
@@ -1186,7 +1193,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="1"/>
@@ -1199,7 +1206,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1224,7 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="F24" s="7">
         <f t="shared" si="0"/>
@@ -1244,7 +1251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1258,14 +1265,14 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12">
         <f>SUM(C24,E24,G24,I24,K24)</f>
-        <v>9.5</v>
+        <v>13.1</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="10" t="s">
         <v>29</v>
       </c>
@@ -1312,12 +1319,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1025" width="10.7109375"/>
   </cols>
@@ -1328,12 +1335,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1025" width="10.7109375"/>
   </cols>

</xml_diff>